<commit_message>
Corrections to commit shas and patches
</commit_message>
<xml_diff>
--- a/CS563-Project/Project/BugComparison/Cs563ProjectFinalBenchmark.xlsx
+++ b/CS563-Project/Project/BugComparison/Cs563ProjectFinalBenchmark.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyesjoshi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyesjoshi/Downloads/CS563-Project/CS563-Project/Project/BugComparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C8A248-CA90-464A-A9C5-916E87820E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1259E434-192D-2548-B327-BA4E5B28C32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13940" yWindow="760" windowWidth="16300" windowHeight="17440" xr2:uid="{807FB612-CEF4-2B43-9A20-8DABEAB288AE}"/>
+    <workbookView xWindow="-38400" yWindow="-13440" windowWidth="38400" windowHeight="21120" xr2:uid="{807FB612-CEF4-2B43-9A20-8DABEAB288AE}"/>
   </bookViews>
   <sheets>
     <sheet name="bug_issues" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="121">
   <si>
     <t>serial_number</t>
   </si>
@@ -263,9 +263,6 @@
     <t>a317ba40fae8e2b11eecde01ad5e6ee15aebdb0f</t>
   </si>
   <si>
-    <t>6978d726971346e6ceb4d0f6da07f066c08bb621</t>
-  </si>
-  <si>
     <t>d50665633b33d84069ccfbeb6a31eeca664d3639</t>
   </si>
   <si>
@@ -278,12 +275,6 @@
     <t>ae5b558ed044be6c9f24197970f43cfcd4fdfaf4</t>
   </si>
   <si>
-    <t>6fc5288a8ed2af7fedda858da17b03927d9c4945</t>
-  </si>
-  <si>
-    <t>fa7747b2b090951be6a62cfcc13a75fdddcd4f40</t>
-  </si>
-  <si>
     <t>e253ce8e2b518aae79d9db13ccfb5b21118cd076</t>
   </si>
   <si>
@@ -296,51 +287,21 @@
     <t>6b403bc21e4bfe0b10f54c12539b34cc761ce5eb</t>
   </si>
   <si>
-    <t>e95b47c8a83b584d24bdfcb6f922ad99b06c135d</t>
-  </si>
-  <si>
-    <t>c614777b7ac1e02258ca2695150dff0fb88fc97b</t>
-  </si>
-  <si>
-    <t>93f8223c3e0764261b8492c8868788de52b2e027</t>
-  </si>
-  <si>
-    <t>eb44c91fbee3bc38f869c088814a2a623b831b3d</t>
-  </si>
-  <si>
     <t>b37caea199031f433ae583e1980811c991b9dd83</t>
   </si>
   <si>
-    <t>d899a1eb1bc83d67cc9ebe0ec74195b0f11f6346</t>
-  </si>
-  <si>
-    <t>62851a9006a686c90d0c27465366e5910d2a93d2</t>
-  </si>
-  <si>
-    <t>2c809b711b0d6a6143ef1ba056235c06b51111ec</t>
-  </si>
-  <si>
     <t>e9c7bb73fb99519d4c38f824dd927687a6426466</t>
   </si>
   <si>
-    <t>6bcdfbd1074f81d615a152be020c6cedcafe21a3</t>
-  </si>
-  <si>
     <t>70682fdee667a36d82f3a81675ac517a196048d9</t>
   </si>
   <si>
-    <t>073db36f3368bfdac22a82cb2f7bcfb76410d497</t>
-  </si>
-  <si>
     <t>44c01dccf285b2b1b494f0764f8f0f8bc987c362</t>
   </si>
   <si>
     <t>b09c1ca3009288b689ff62d7fdd3c5624dd17091</t>
   </si>
   <si>
-    <t>05c4a4840c4f007790895298ed48567a6d0c3c81</t>
-  </si>
-  <si>
     <t>b8f662f59ea24eaf2f5f682dbece6c9fd1053354</t>
   </si>
   <si>
@@ -350,43 +311,94 @@
     <t>7a476ce54432bbe8cd7fc6429faa7dd487914251</t>
   </si>
   <si>
-    <t>0fd53d3aec17e1adeddd04a57ccb7231410d4d92</t>
-  </si>
-  <si>
-    <t>2dd0f74a90667862262e67fa06989dd8a47e87a6</t>
-  </si>
-  <si>
-    <t>b8f4cbbbb75d6562f13f49ec5d29c156a1e42d47</t>
-  </si>
-  <si>
-    <t>c52d5f8731b46cdbd502f693a39247fe48543d34</t>
-  </si>
-  <si>
-    <t>10f929230b397c42676d3fd506281a6b63e04643</t>
-  </si>
-  <si>
     <t>457947102a8568255d0dfb2161a17d646d7d6e25</t>
   </si>
   <si>
     <t>c54cd1bedacefd0eac5674fff932fddd2e5c2232</t>
   </si>
   <si>
-    <t>ae33581c3f2b1a0cc4f49caa87fbb1ffa69659a5</t>
-  </si>
-  <si>
-    <t>9b28eb2e2defc99594ae647835cd448bf5727496</t>
-  </si>
-  <si>
-    <t>35a0292d7ebb956082b389fc2fe18a9ae09a9a98</t>
-  </si>
-  <si>
-    <t>f575c31aa737ac6fcf7ec89862c255a02d818687</t>
-  </si>
-  <si>
-    <t>9d6243f9af437f0af59d52d9eff38594d419a95d</t>
-  </si>
-  <si>
-    <t>947e3d95fe6b61c8a0749956b323e2ed845bc430</t>
+    <t>d61e392c770713344b81b443f8742635ccca6785</t>
+  </si>
+  <si>
+    <t>736019f4ebc413002f490223257ccb454978fe06</t>
+  </si>
+  <si>
+    <t>51d5bdba89b39d1cb4326e57b91ece315133b319</t>
+  </si>
+  <si>
+    <t>4b07190045d033edf90deecbae0a4a0edf913f6e</t>
+  </si>
+  <si>
+    <t>b1c1e847131fdb43c0cb605cf5f99077f4568ce5</t>
+  </si>
+  <si>
+    <t>1b49280ada50122c64f1932b72613afc4566a213</t>
+  </si>
+  <si>
+    <t>a994bf2f6b14d7dfadb00558ed6fd65709e166c3</t>
+  </si>
+  <si>
+    <t>c1d8b864ece8c3188fd13e0bfd099a08759d9b89</t>
+  </si>
+  <si>
+    <t>e6e5ce634c20f04ce9779bcc6587d9196fdfee25</t>
+  </si>
+  <si>
+    <t>f0fd25088cbeedc76dc4f0220298b90b0ee613ed</t>
+  </si>
+  <si>
+    <t>000fa18ed78f00b96206404f085838bc070142c4</t>
+  </si>
+  <si>
+    <t>d6786945002431e73874bab7f191f919b4b21360</t>
+  </si>
+  <si>
+    <t>2220e0620c70d82aa209d1431f5e4fa8105b1e09</t>
+  </si>
+  <si>
+    <t>17eb109be3c831ec8fc96261c07711add1e448f4</t>
+  </si>
+  <si>
+    <t>1a57f43231b49988ecc40f27d493e20575b5db6a</t>
+  </si>
+  <si>
+    <t>6618eb0d2267806eb7bc42ba61fb8be3ad2e50ca</t>
+  </si>
+  <si>
+    <t>346cdb9d3f825b8cf1b396adf511a2909975f778</t>
+  </si>
+  <si>
+    <t>c712665c6b407852788db6d208644417849b7660</t>
+  </si>
+  <si>
+    <t>eca1187e5e7b7187284b1db8e080c8ec76c50269</t>
+  </si>
+  <si>
+    <t>2209c8114e38c909614c2a2a5b5b02d80082a7d6</t>
+  </si>
+  <si>
+    <t>7e349c536046f93dae6a79ef7747374fc1d303ad</t>
+  </si>
+  <si>
+    <t>1efcba2162fad2b86ef546113e8881c5b809b47f</t>
+  </si>
+  <si>
+    <t>2041d2b33e2c4dc55d9d87478e3b2c926e8aa579</t>
+  </si>
+  <si>
+    <t>a8856c90c53a10410eaeeae91f5c31173f1e49d6</t>
+  </si>
+  <si>
+    <t>a0a700f810848477e0189dbea2ea41df5db78e6e</t>
+  </si>
+  <si>
+    <t>b63aa0aa999f18587fd96b14b99f92d9ac67b0cf</t>
+  </si>
+  <si>
+    <t>When an update is made, the version of a record is incremented. However, some functionalities exclusively search for records with version zero.</t>
+  </si>
+  <si>
+    <t>A test fails on some systems because of a concurrency issue.</t>
   </si>
 </sst>
 </file>
@@ -416,18 +428,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -443,14 +449,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -788,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AE2BB3-8133-5D4A-B3A2-E7390600A9FE}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -855,11 +864,11 @@
       <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>75</v>
+      <c r="J2" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -881,11 +890,11 @@
       <c r="H3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>76</v>
+      <c r="I3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -907,11 +916,11 @@
       <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -933,11 +942,11 @@
       <c r="H5" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>80</v>
+      <c r="I5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -959,11 +968,11 @@
       <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>82</v>
+      <c r="I6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -985,33 +994,39 @@
       <c r="H7" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>83</v>
+      <c r="I7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="114" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>85</v>
+      <c r="D8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1033,11 +1048,11 @@
       <c r="H9" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>86</v>
+      <c r="I9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1059,11 +1074,11 @@
       <c r="H10" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>85</v>
+      <c r="I10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1085,11 +1100,11 @@
       <c r="H11" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>88</v>
+      <c r="I11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1111,11 +1126,11 @@
       <c r="H12" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>90</v>
+      <c r="I12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1137,11 +1152,11 @@
       <c r="H13" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>92</v>
+      <c r="I13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1163,11 +1178,11 @@
       <c r="H14" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>94</v>
+      <c r="I14" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1189,11 +1204,11 @@
       <c r="H15" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>96</v>
+      <c r="I15" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1215,11 +1230,11 @@
       <c r="H16" t="s">
         <v>51</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>98</v>
+      <c r="I16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1241,11 +1256,11 @@
       <c r="H17" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>100</v>
+      <c r="I17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1264,11 +1279,14 @@
       <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>102</v>
+      <c r="H18" t="s">
+        <v>120</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1290,11 +1308,11 @@
       <c r="H19" t="s">
         <v>57</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>104</v>
+      <c r="I19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1316,11 +1334,11 @@
       <c r="H20" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>106</v>
+      <c r="I20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1342,11 +1360,11 @@
       <c r="H21" t="s">
         <v>61</v>
       </c>
-      <c r="I21" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>108</v>
+      <c r="I21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1368,11 +1386,11 @@
       <c r="H22" t="s">
         <v>63</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>110</v>
+      <c r="I22" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1394,11 +1412,11 @@
       <c r="H23" t="s">
         <v>65</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>112</v>
+      <c r="I23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1420,11 +1438,11 @@
       <c r="H24" t="s">
         <v>67</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>114</v>
+      <c r="I24" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="114" x14ac:dyDescent="0.2">
@@ -1446,11 +1464,11 @@
       <c r="H25" t="s">
         <v>70</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>116</v>
+      <c r="I25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>